<commit_message>
Modified class for 8828, removed obsolet functions adjusted existing for 8828, added save_histograms. Also added new spreadsheet page with 8828 registers
</commit_message>
<xml_diff>
--- a/python/Registers.xlsx
+++ b/python/Registers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koer2434\Documents\fpga\pyripherals\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gamm5831\Documents\FPGA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE2DF48-9317-4225-87D8-771B41E9424E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2300323F-B5D9-4174-9345-AE0EA578E711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="9" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="11" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
   </bookViews>
   <sheets>
     <sheet name="I2C" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="341">
   <si>
     <t>Name</t>
   </si>
@@ -1054,6 +1054,24 @@
   </si>
   <si>
     <t>0xD</t>
+  </si>
+  <si>
+    <t>8828AKG_SETTINGS</t>
+  </si>
+  <si>
+    <t>8828HIST_DUMP</t>
+  </si>
+  <si>
+    <t>8828ACTIVE_RANGE</t>
+  </si>
+  <si>
+    <t>0x19</t>
+  </si>
+  <si>
+    <t>0x6F</t>
+  </si>
+  <si>
+    <t>8828SPAD_MAP_ID</t>
   </si>
 </sst>
 </file>
@@ -1593,8 +1611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1CC0846-B885-4A4F-9321-B09606FEAD42}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2774,10 +2792,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664851F3-DE29-D040-BC28-9A1DBE9A5B1C}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3623,6 +3641,86 @@
         <v>7</v>
       </c>
       <c r="F42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>335</v>
+      </c>
+      <c r="B43" t="s">
+        <v>254</v>
+      </c>
+      <c r="C43" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43">
+        <v>8</v>
+      </c>
+      <c r="E43">
+        <v>7</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>336</v>
+      </c>
+      <c r="B44" t="s">
+        <v>262</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44">
+        <v>8</v>
+      </c>
+      <c r="E44">
+        <v>7</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>337</v>
+      </c>
+      <c r="B45" t="s">
+        <v>338</v>
+      </c>
+      <c r="C45" t="s">
+        <v>339</v>
+      </c>
+      <c r="D45">
+        <v>8</v>
+      </c>
+      <c r="E45">
+        <v>7</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>340</v>
+      </c>
+      <c r="B46" t="s">
+        <v>252</v>
+      </c>
+      <c r="C46" t="s">
+        <v>56</v>
+      </c>
+      <c r="D46">
+        <v>4</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="F46">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made modifications to copy of 8801 one class to use new 8828 spreadsheeet page and update functions
</commit_message>
<xml_diff>
--- a/python/Registers.xlsx
+++ b/python/Registers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gamm5831\Documents\FPGA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gamm5831\Documents\FPGA\pyripherals\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2300323F-B5D9-4174-9345-AE0EA578E711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7238908-ED16-413A-8A4A-A907D2D278F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="11" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="12" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
   </bookViews>
   <sheets>
     <sheet name="I2C" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,8 @@
     <sheet name="ADS8686" sheetId="16" r:id="rId10"/>
     <sheet name="AD7961" sheetId="13" r:id="rId11"/>
     <sheet name="TMF8801" sheetId="17" r:id="rId12"/>
-    <sheet name="DAC101C081" sheetId="18" r:id="rId13"/>
+    <sheet name="TMF8828" sheetId="19" r:id="rId13"/>
+    <sheet name="DAC101C081" sheetId="18" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">I2C!$A$1:$E$6</definedName>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="390">
   <si>
     <t>Name</t>
   </si>
@@ -1056,22 +1057,169 @@
     <t>0xD</t>
   </si>
   <si>
-    <t>8828AKG_SETTINGS</t>
-  </si>
-  <si>
-    <t>8828HIST_DUMP</t>
-  </si>
-  <si>
-    <t>8828ACTIVE_RANGE</t>
-  </si>
-  <si>
-    <t>0x19</t>
-  </si>
-  <si>
-    <t>0x6F</t>
-  </si>
-  <si>
-    <t>8828SPAD_MAP_ID</t>
+    <t>0X00</t>
+  </si>
+  <si>
+    <t>MINOR</t>
+  </si>
+  <si>
+    <t>0X01</t>
+  </si>
+  <si>
+    <t>0XE0</t>
+  </si>
+  <si>
+    <t>0XE1</t>
+  </si>
+  <si>
+    <t>0XE2</t>
+  </si>
+  <si>
+    <t>0XE3</t>
+  </si>
+  <si>
+    <t>0XE4</t>
+  </si>
+  <si>
+    <t>0X08</t>
+  </si>
+  <si>
+    <t>PATCH</t>
+  </si>
+  <si>
+    <t>0X02</t>
+  </si>
+  <si>
+    <t>BUILD_TYPE</t>
+  </si>
+  <si>
+    <t>0X03</t>
+  </si>
+  <si>
+    <t>APPLICATION_STATUS</t>
+  </si>
+  <si>
+    <t>0X04</t>
+  </si>
+  <si>
+    <t>MEASURE_STATUS</t>
+  </si>
+  <si>
+    <t>0X05</t>
+  </si>
+  <si>
+    <t>ALGORITHM_STATUS</t>
+  </si>
+  <si>
+    <t>0X06</t>
+  </si>
+  <si>
+    <t>CALIBRATION_STATUS</t>
+  </si>
+  <si>
+    <t>0X07</t>
+  </si>
+  <si>
+    <t>CMD_STAT</t>
+  </si>
+  <si>
+    <t>PREV_CMD</t>
+  </si>
+  <si>
+    <t>0X09</t>
+  </si>
+  <si>
+    <t>MODE</t>
+  </si>
+  <si>
+    <t>0X10</t>
+  </si>
+  <si>
+    <t>LIVE_BEAT</t>
+  </si>
+  <si>
+    <t>0X0A</t>
+  </si>
+  <si>
+    <t>ACTIVE_RANGE</t>
+  </si>
+  <si>
+    <t>0X19</t>
+  </si>
+  <si>
+    <t>0X6F</t>
+  </si>
+  <si>
+    <t>CONFIG_RESULT</t>
+  </si>
+  <si>
+    <t>0X21</t>
+  </si>
+  <si>
+    <t>SIZE</t>
+  </si>
+  <si>
+    <t>0X22</t>
+  </si>
+  <si>
+    <t>PERIOD</t>
+  </si>
+  <si>
+    <t>0X24</t>
+  </si>
+  <si>
+    <t>0X219</t>
+  </si>
+  <si>
+    <t>KILO_ITERATIONS</t>
+  </si>
+  <si>
+    <t>0X26</t>
+  </si>
+  <si>
+    <t>CONFIDENCE_THRESHOLD</t>
+  </si>
+  <si>
+    <t>0X30</t>
+  </si>
+  <si>
+    <t>ALG_SETTING</t>
+  </si>
+  <si>
+    <t>SPAD_MAP_ID</t>
+  </si>
+  <si>
+    <t>HIST_DUMP</t>
+  </si>
+  <si>
+    <t>SPREAD_SPECTRUM</t>
+  </si>
+  <si>
+    <t>0X3A</t>
+  </si>
+  <si>
+    <t>I2C_SLAVE_ADDRESS</t>
+  </si>
+  <si>
+    <t>0X3B</t>
+  </si>
+  <si>
+    <t>0X41</t>
+  </si>
+  <si>
+    <t>OSC_TRIM_VALUE</t>
+  </si>
+  <si>
+    <t>0X3C</t>
+  </si>
+  <si>
+    <t>I2C_ADDR_CHANGE</t>
+  </si>
+  <si>
+    <t>0X3E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                                                  </t>
   </si>
 </sst>
 </file>
@@ -2792,10 +2940,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664851F3-DE29-D040-BC28-9A1DBE9A5B1C}">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3644,92 +3792,721 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>335</v>
-      </c>
-      <c r="B43" t="s">
-        <v>254</v>
-      </c>
-      <c r="C43" t="s">
-        <v>30</v>
-      </c>
-      <c r="D43">
-        <v>8</v>
-      </c>
-      <c r="E43">
-        <v>7</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>336</v>
-      </c>
-      <c r="B44" t="s">
-        <v>262</v>
-      </c>
-      <c r="C44" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44">
-        <v>8</v>
-      </c>
-      <c r="E44">
-        <v>7</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>337</v>
-      </c>
-      <c r="B45" t="s">
-        <v>338</v>
-      </c>
-      <c r="C45" t="s">
-        <v>339</v>
-      </c>
-      <c r="D45">
-        <v>8</v>
-      </c>
-      <c r="E45">
-        <v>7</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>340</v>
-      </c>
-      <c r="B46" t="s">
-        <v>252</v>
-      </c>
-      <c r="C46" t="s">
-        <v>56</v>
-      </c>
-      <c r="D46">
-        <v>4</v>
-      </c>
-      <c r="E46">
-        <v>3</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{072B7DE6-307C-4EEA-96B3-5B6831C6A020}">
+  <dimension ref="A1:F35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>336</v>
+      </c>
+      <c r="B3" t="s">
+        <v>337</v>
+      </c>
+      <c r="C3" t="s">
+        <v>335</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>278</v>
+      </c>
+      <c r="B4" t="s">
+        <v>338</v>
+      </c>
+      <c r="C4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>322</v>
+      </c>
+      <c r="B5" t="s">
+        <v>279</v>
+      </c>
+      <c r="C5" t="s">
+        <v>335</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>323</v>
+      </c>
+      <c r="B6" t="s">
+        <v>279</v>
+      </c>
+      <c r="C6" t="s">
+        <v>335</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>280</v>
+      </c>
+      <c r="B7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C7" t="s">
+        <v>335</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B8" t="s">
+        <v>340</v>
+      </c>
+      <c r="C8" t="s">
+        <v>335</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" t="s">
+        <v>341</v>
+      </c>
+      <c r="C9" t="s">
+        <v>343</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>285</v>
+      </c>
+      <c r="B10" t="s">
+        <v>342</v>
+      </c>
+      <c r="C10" t="s">
+        <v>335</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>344</v>
+      </c>
+      <c r="B11" t="s">
+        <v>345</v>
+      </c>
+      <c r="C11" t="s">
+        <v>335</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>7</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>346</v>
+      </c>
+      <c r="B12" t="s">
+        <v>347</v>
+      </c>
+      <c r="C12" t="s">
+        <v>335</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>348</v>
+      </c>
+      <c r="B13" t="s">
+        <v>349</v>
+      </c>
+      <c r="C13" t="s">
+        <v>335</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>7</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>350</v>
+      </c>
+      <c r="B14" t="s">
+        <v>351</v>
+      </c>
+      <c r="C14" t="s">
+        <v>335</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>352</v>
+      </c>
+      <c r="B15" t="s">
+        <v>353</v>
+      </c>
+      <c r="C15" t="s">
+        <v>335</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>7</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>354</v>
+      </c>
+      <c r="B16" t="s">
+        <v>355</v>
+      </c>
+      <c r="C16" t="s">
+        <v>335</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>356</v>
+      </c>
+      <c r="B17" t="s">
+        <v>343</v>
+      </c>
+      <c r="C17" t="s">
+        <v>335</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>357</v>
+      </c>
+      <c r="B18" t="s">
+        <v>358</v>
+      </c>
+      <c r="C18" t="s">
+        <v>335</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>359</v>
+      </c>
+      <c r="B19" t="s">
+        <v>360</v>
+      </c>
+      <c r="C19" t="s">
+        <v>335</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <v>7</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>361</v>
+      </c>
+      <c r="B20" t="s">
+        <v>362</v>
+      </c>
+      <c r="C20" t="s">
+        <v>335</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+      <c r="E20">
+        <v>7</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>363</v>
+      </c>
+      <c r="B21" t="s">
+        <v>364</v>
+      </c>
+      <c r="C21" t="s">
+        <v>365</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>7</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>366</v>
+      </c>
+      <c r="B22" t="s">
+        <v>185</v>
+      </c>
+      <c r="C22" t="s">
+        <v>335</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>319</v>
+      </c>
+      <c r="B23" t="s">
+        <v>367</v>
+      </c>
+      <c r="C23" t="s">
+        <v>335</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="E23">
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>368</v>
+      </c>
+      <c r="B24" t="s">
+        <v>369</v>
+      </c>
+      <c r="C24" t="s">
+        <v>335</v>
+      </c>
+      <c r="D24">
+        <v>16</v>
+      </c>
+      <c r="E24">
+        <v>15</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>370</v>
+      </c>
+      <c r="B25" t="s">
+        <v>371</v>
+      </c>
+      <c r="C25" t="s">
+        <v>367</v>
+      </c>
+      <c r="D25">
+        <v>16</v>
+      </c>
+      <c r="E25">
+        <v>15</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>373</v>
+      </c>
+      <c r="B26" t="s">
+        <v>374</v>
+      </c>
+      <c r="C26" t="s">
+        <v>372</v>
+      </c>
+      <c r="D26">
+        <v>16</v>
+      </c>
+      <c r="E26">
+        <v>15</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>375</v>
+      </c>
+      <c r="B27" t="s">
+        <v>376</v>
+      </c>
+      <c r="C27" t="s">
+        <v>353</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="E27">
+        <v>7</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>378</v>
+      </c>
+      <c r="B28" t="s">
+        <v>252</v>
+      </c>
+      <c r="C28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>377</v>
+      </c>
+      <c r="B29" t="s">
+        <v>254</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29">
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <v>7</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>379</v>
+      </c>
+      <c r="B30" t="s">
+        <v>262</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30">
+        <v>8</v>
+      </c>
+      <c r="E30">
+        <v>7</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>380</v>
+      </c>
+      <c r="B31" t="s">
+        <v>381</v>
+      </c>
+      <c r="C31" t="s">
+        <v>335</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>382</v>
+      </c>
+      <c r="B32" t="s">
+        <v>383</v>
+      </c>
+      <c r="C32" t="s">
+        <v>384</v>
+      </c>
+      <c r="D32">
+        <v>7</v>
+      </c>
+      <c r="E32">
+        <v>7</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>385</v>
+      </c>
+      <c r="B33" t="s">
+        <v>386</v>
+      </c>
+      <c r="C33" t="s">
+        <v>335</v>
+      </c>
+      <c r="D33">
+        <v>9</v>
+      </c>
+      <c r="E33">
+        <v>8</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>387</v>
+      </c>
+      <c r="B34" t="s">
+        <v>388</v>
+      </c>
+      <c r="C34" t="s">
+        <v>335</v>
+      </c>
+      <c r="D34">
+        <v>8</v>
+      </c>
+      <c r="E34">
+        <v>7</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>389</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88D16BBE-84DB-394B-A8D9-7783FA0567DF}">
   <dimension ref="A1:F3"/>
   <sheetViews>

</xml_diff>

<commit_message>
update I2CController for repeater
</commit_message>
<xml_diff>
--- a/python/Registers.xlsx
+++ b/python/Registers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lloy7803\Documents\pyripherals\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B764526E-A9C9-4E4A-9F66-722E91FACA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9DB4C44-8290-4AD0-A5DF-FB33253FEAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" firstSheet="6" activeTab="12" xr2:uid="{C3AB243F-651F-4CB0-B6E1-3CA4785EC4D9}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="391">
   <si>
     <t>Name</t>
   </si>
@@ -1217,6 +1217,12 @@
   </si>
   <si>
     <t>0X3E</t>
+  </si>
+  <si>
+    <t>POWER_CFG</t>
+  </si>
+  <si>
+    <t>0X33</t>
   </si>
 </sst>
 </file>
@@ -3796,10 +3802,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{072B7DE6-307C-4EEA-96B3-5B6831C6A020}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4489,6 +4495,26 @@
         <v>7</v>
       </c>
       <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>389</v>
+      </c>
+      <c r="B35" t="s">
+        <v>390</v>
+      </c>
+      <c r="C35" t="s">
+        <v>335</v>
+      </c>
+      <c r="D35">
+        <v>8</v>
+      </c>
+      <c r="E35">
+        <v>7</v>
+      </c>
+      <c r="F35">
         <v>0</v>
       </c>
     </row>

</xml_diff>